<commit_message>
Did a non-regex approach
</commit_message>
<xml_diff>
--- a/CH-98 Data Cleaning.xlsx
+++ b/CH-98 Data Cleaning.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE93C491-B1B9-4966-9CCB-EDDF81375A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FF7004-1AF2-4729-9AA9-1065D71A4093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$B$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$B$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$B$9</definedName>
   </definedNames>
@@ -42,8 +44,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -54,16 +57,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="24">
   <si>
     <t>Question</t>
   </si>
@@ -129,6 +146,12 @@
   </si>
   <si>
     <t>Early had the classic solution</t>
+  </si>
+  <si>
+    <t>https://youtu.be/DN4gjmsZpcY</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -664,6 +687,68 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>A</v>
+    <v>2</v>
+    <v>5</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="argument" t="s"/>
+    <k n="errorType" t="i"/>
+    <k n="ptg" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Dividend">
   <a:themeElements>
@@ -933,6 +1018,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="9">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{5C163C9C-10FD-47D8-A852-FF88D1DE669D}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J22"/>
@@ -1171,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B29CFA9-06D0-4E39-952A-51C93B41058E}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -1475,4 +1587,358 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2169B5C2-11FD-49F8-BBD9-21879110A4D8}">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="2"/>
+      <c r="J1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" s="8">
+        <v>45386</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9">
+        <v>10</v>
+      </c>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4" s="8">
+        <v>45395</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="9">
+        <v>2</v>
+      </c>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5" s="8">
+        <v>45397</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="10">
+        <v>4</v>
+      </c>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6" s="8">
+        <v>45404</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="9">
+        <v>3</v>
+      </c>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7" s="8">
+        <v>45412</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="9">
+        <v>2</v>
+      </c>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8" s="8">
+        <v>45416</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="9">
+        <v>3</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9" s="8">
+        <v>45419</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="9">
+        <v>5</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="3"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11"/>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="3"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B13" s="3" t="str" cm="1">
+        <f t="array" ref="B13:D20">_xlfn.REDUCE(
+    _xlfn.HSTACK("Date", "Product", "Quantity"),
+    B3:B9,
+    _xlfn.LAMBDA(_xlpm.A,_xlpm.B,
+        _xlfn.VSTACK(
+            _xlpm.A,
+            _xlfn.LET(
+                _xlpm.S, TRIM(_xlfn.TEXTSPLIT(_xlpm.B, ",")),
+                _xlpm.O, _xlfn._xlws.SORT(IFERROR(_xlpm.S * 1, _xlpm.S), , , 1),
+                _xlfn.HSTACK(_xlfn.CHOOSECOLS(_xlpm.O, 2), _xlfn.TAKE(_xlpm.O, , -1), _xlfn.TAKE(_xlpm.O, , 1))
+            )
+        )
+    )
+)</f>
+        <v>Date</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Product</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Quantity</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B14" s="3">
+        <v>45386</v>
+      </c>
+      <c r="C14" t="str">
+        <v>A</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="G14" t="str" cm="1">
+        <f t="array" ref="G14:I14">TRIM(_xlfn.TEXTSPLIT(B3, ","))</f>
+        <v>2024/04/04</v>
+      </c>
+      <c r="H14" t="str">
+        <v>10</v>
+      </c>
+      <c r="I14" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3">
+        <v>45395</v>
+      </c>
+      <c r="C15" t="str">
+        <v>M</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="G15" cm="1">
+        <f t="array" ref="G15:I15">_xlfn._xlws.SORT(IFERROR(_xlfn.ANCHORARRAY(G14) * 1,_xlfn.ANCHORARRAY( G14)), , , 1)</f>
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>45386</v>
+      </c>
+      <c r="I15" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3">
+        <v>45397</v>
+      </c>
+      <c r="C16" t="str">
+        <v>A</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="G16" cm="1">
+        <f t="array" ref="G16:I16">_xlfn.ANCHORARRAY(G14) * 1</f>
+        <v>45386</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3">
+        <v>45404</v>
+      </c>
+      <c r="C17" t="str">
+        <v>B</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="3">
+        <v>45412</v>
+      </c>
+      <c r="C18" t="str">
+        <v>A</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3">
+        <v>45416</v>
+      </c>
+      <c r="C19" t="str">
+        <v>AB</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="3">
+        <v>45419</v>
+      </c>
+      <c r="C20" t="str">
+        <v>AB</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A22" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>